<commit_message>
More EB fixes, some documentation added, pre high res model setup
</commit_message>
<xml_diff>
--- a/SATIM/DataSpreadsheets/TCH_IND/TCH_IND_PP.xlsx
+++ b/SATIM/DataSpreadsheets/TCH_IND/TCH_IND_PP.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\SATIM\DataSpreadsheets\TCH_IND\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AD38DF-343F-4742-BCD3-0992528F2B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F69BC3-2BE9-4E01-B74C-33BC49AB7142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="721" firstSheet="3" activeTab="3" xr2:uid="{F729A2FB-7487-448B-BFDD-0350B6F47A76}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="721" activeTab="16" xr2:uid="{F729A2FB-7487-448B-BFDD-0350B6F47A76}"/>
+    <workbookView xWindow="28680" yWindow="5355" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{4B7FA444-669B-4756-9286-B93FCE4ED703}"/>
   </bookViews>
   <sheets>
     <sheet name="Worklog" sheetId="61" r:id="rId1"/>
@@ -232,7 +233,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="352">
   <si>
     <t>Comment</t>
   </si>
@@ -1278,6 +1279,27 @@
   </si>
   <si>
     <t>Selected</t>
+  </si>
+  <si>
+    <t>N Gas balance fix. N gas usage is out by a lot in BY. Fixing this</t>
+  </si>
+  <si>
+    <t>NB: There is a lot content in the old workbook "SATIM - industry - P&amp;P - 23June2021"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EB comes from the old workbook "SATIM - industry - P&amp;P - 23June2021" which is based on Tamaryn's work. </t>
+  </si>
+  <si>
+    <t>steam gen</t>
+  </si>
+  <si>
+    <t>steam use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have dropped the outputs in order to calibrate the EB. </t>
+  </si>
+  <si>
+    <t>NCAP_AFA-LO</t>
   </si>
 </sst>
 </file>
@@ -1295,7 +1317,7 @@
     <numFmt numFmtId="170" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="50" x14ac:knownFonts="1">
+  <fonts count="51" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1624,8 +1646,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1663,6 +1691,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9E1F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2083,7 +2117,7 @@
     <xf numFmtId="43" fontId="43" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="233">
+  <cellXfs count="242">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2501,6 +2535,23 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Bad" xfId="21" builtinId="27"/>
@@ -3166,9 +3217,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>247650</xdr:colOff>
+          <xdr:colOff>238125</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
+          <xdr:rowOff>104775</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3224,9 +3275,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>238125</xdr:colOff>
+          <xdr:colOff>228600</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3282,9 +3333,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>247650</xdr:colOff>
+          <xdr:colOff>238125</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3340,9 +3391,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>581025</xdr:colOff>
+          <xdr:colOff>571500</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3398,9 +3449,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:colOff>552450</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3519,7 +3570,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
@@ -3756,7 +3807,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>1933575</xdr:colOff>
+          <xdr:colOff>1924050</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3935,7 +3986,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1314450</xdr:colOff>
+          <xdr:colOff>1304925</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -4346,7 +4397,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>857250</xdr:colOff>
+          <xdr:colOff>847725</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -5168,7 +5219,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>847725</xdr:colOff>
+          <xdr:colOff>838200</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
@@ -6222,7 +6273,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>95250</xdr:rowOff>
         </xdr:to>
@@ -6809,7 +6860,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>819150</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7990,7 +8041,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>847725</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
+          <xdr:rowOff>104775</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -8575,7 +8626,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
+          <xdr:rowOff>104775</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -9629,7 +9680,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>666750</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -9936,7 +9987,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:to>
@@ -9999,7 +10050,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>1933575</xdr:colOff>
+          <xdr:colOff>1924050</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -10178,7 +10229,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>1933575</xdr:colOff>
+          <xdr:colOff>1924050</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -10357,7 +10408,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>1933575</xdr:colOff>
+          <xdr:colOff>1924050</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -10773,7 +10824,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
@@ -11345,17 +11396,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5684EB7D-CDEE-4A87-AF47-0484D2008B77}">
-  <dimension ref="A6:C11"/>
+  <dimension ref="A2:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="59.140625" style="185" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="234" t="s">
+        <v>346</v>
+      </c>
+    </row>
     <row r="6" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="185" t="s">
         <v>236</v>
@@ -11382,8 +11439,20 @@
         <v>341</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="185" t="s">
+        <v>345</v>
+      </c>
+      <c r="B15" s="233">
+        <v>44603</v>
+      </c>
+      <c r="C15" t="s">
+        <v>304</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11397,6 +11466,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11727,7 +11797,7 @@
               </from>
               <to>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>1933575</xdr:colOff>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -11749,6 +11819,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11870,7 +11941,7 @@
               </from>
               <to>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>1933575</xdr:colOff>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -11892,6 +11963,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12016,9 +12088,9 @@
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>581025</xdr:colOff>
+                <xdr:colOff>571500</xdr:colOff>
                 <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>28575</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -12038,6 +12110,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12095,7 +12168,7 @@
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>28575</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -12143,7 +12216,7 @@
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>47625</xdr:rowOff>
               </to>
@@ -12219,6 +12292,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4:K13"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12481,7 +12555,7 @@
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>47625</xdr:rowOff>
               </to>
@@ -12529,9 +12603,10 @@
   </sheetPr>
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F50" sqref="F50"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13336,7 +13411,7 @@
               </from>
               <to>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>1933575</xdr:colOff>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -13358,6 +13433,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13437,7 +13513,7 @@
               </from>
               <to>
                 <xdr:col>2</xdr:col>
-                <xdr:colOff>1314450</xdr:colOff>
+                <xdr:colOff>1304925</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -13462,7 +13538,7 @@
               </from>
               <to>
                 <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:colOff>28575</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -13608,14 +13684,15 @@
   <sheetPr codeName="Sheet30">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:AX89"/>
+  <dimension ref="A1:AZ89"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="L70" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="W100" sqref="W100"/>
+      <selection pane="bottomRight" activeCell="V40" sqref="V40"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13627,14 +13704,14 @@
     <col min="6" max="6" width="10.140625" style="12" customWidth="1"/>
     <col min="7" max="7" width="6.85546875" style="45" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="31" width="9.140625" style="12"/>
-    <col min="32" max="32" width="7.85546875" style="12" customWidth="1"/>
-    <col min="33" max="33" width="7.5703125" style="12" customWidth="1"/>
-    <col min="34" max="35" width="7.85546875" style="12" customWidth="1"/>
-    <col min="37" max="16384" width="9.140625" style="12"/>
+    <col min="9" max="33" width="9.140625" style="12"/>
+    <col min="34" max="34" width="7.85546875" style="12" customWidth="1"/>
+    <col min="35" max="35" width="7.5703125" style="12" customWidth="1"/>
+    <col min="36" max="37" width="7.85546875" style="12" customWidth="1"/>
+    <col min="39" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="str">
         <f ca="1">IF(INDEX(Index!$E$6:$E$37,MATCH(A2,Index!$D$6:$D$37,0))=1,LEFT(A2,SEARCH("_",A2)-1),"")</f>
         <v>ProcData</v>
@@ -13644,14 +13721,6 @@
         <v>REGION1</v>
       </c>
       <c r="H1" s="53"/>
-      <c r="AQ1" s="199" t="str">
-        <f>IF('PAMS levers'!$B$2,"","*")</f>
-        <v/>
-      </c>
-      <c r="AR1" s="199" t="str">
-        <f>IF('PAMS levers'!$B$2,"","*")</f>
-        <v/>
-      </c>
       <c r="AS1" s="199" t="str">
         <f>IF('PAMS levers'!$B$2,"","*")</f>
         <v/>
@@ -13676,8 +13745,16 @@
         <f>IF('PAMS levers'!$B$2,"","*")</f>
         <v/>
       </c>
-    </row>
-    <row r="2" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AY1" s="199" t="str">
+        <f>IF('PAMS levers'!$B$2,"","*")</f>
+        <v/>
+      </c>
+      <c r="AZ1" s="199" t="str">
+        <f>IF('PAMS levers'!$B$2,"","*")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f ca="1">MID(CELL("filename",A2),FIND("]",CELL("filename",A2))+1,255)</f>
         <v>ProcData_plants and boilers</v>
@@ -13694,7 +13771,7 @@
       <c r="O2" s="53"/>
       <c r="P2" s="53"/>
     </row>
-    <row r="3" spans="1:50" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22"/>
       <c r="H3" s="104" t="s">
         <v>148</v>
@@ -13736,32 +13813,34 @@
       <c r="U3" s="104"/>
       <c r="V3" s="104"/>
       <c r="W3" s="104"/>
-      <c r="X3" s="12" t="s">
+      <c r="X3" s="104"/>
+      <c r="Y3" s="104"/>
+      <c r="Z3" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="Y3" s="12" t="s">
+      <c r="AA3" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="Z3" s="104" t="s">
+      <c r="AB3" s="104" t="s">
         <v>158</v>
       </c>
-      <c r="AA3" s="104" t="s">
+      <c r="AC3" s="104" t="s">
         <v>159</v>
       </c>
-      <c r="AB3" s="104" t="s">
+      <c r="AD3" s="104" t="s">
         <v>159</v>
       </c>
-      <c r="AC3" s="104"/>
-      <c r="AD3" s="104"/>
-      <c r="AE3" s="12" t="s">
+      <c r="AE3" s="104"/>
+      <c r="AF3" s="104"/>
+      <c r="AG3" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="AF3" s="12" t="s">
+      <c r="AH3" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="AL3" s="53"/>
-    </row>
-    <row r="4" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN3" s="53"/>
+    </row>
+    <row r="4" spans="1:52" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="22"/>
       <c r="E4" s="46"/>
       <c r="F4" s="46"/>
@@ -13809,40 +13888,40 @@
         <v>230</v>
       </c>
       <c r="V4" s="103" t="s">
+        <v>351</v>
+      </c>
+      <c r="W4" s="103" t="s">
+        <v>351</v>
+      </c>
+      <c r="X4" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="W4" s="103" t="s">
+      <c r="Y4" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="X4" s="103" t="s">
+      <c r="Z4" s="103" t="s">
         <v>231</v>
       </c>
-      <c r="Y4" s="103" t="s">
+      <c r="AA4" s="103" t="s">
         <v>231</v>
-      </c>
-      <c r="Z4" s="103" t="s">
-        <v>142</v>
-      </c>
-      <c r="AA4" s="103" t="s">
-        <v>142</v>
       </c>
       <c r="AB4" s="103" t="s">
         <v>142</v>
       </c>
       <c r="AC4" s="103" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD4" s="103" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE4" s="103" t="s">
         <v>342</v>
       </c>
-      <c r="AD4" s="103" t="s">
+      <c r="AF4" s="103" t="s">
         <v>342</v>
       </c>
-      <c r="AE4" s="26" t="s">
+      <c r="AG4" s="26" t="s">
         <v>128</v>
-      </c>
-      <c r="AF4" s="103" t="s">
-        <v>141</v>
-      </c>
-      <c r="AG4" s="103" t="s">
-        <v>141</v>
       </c>
       <c r="AH4" s="103" t="s">
         <v>141</v>
@@ -13857,16 +13936,16 @@
         <v>141</v>
       </c>
       <c r="AL4" s="103" t="s">
+        <v>141</v>
+      </c>
+      <c r="AM4" s="103" t="s">
+        <v>141</v>
+      </c>
+      <c r="AN4" s="103" t="s">
         <v>168</v>
       </c>
-      <c r="AM4" s="12" t="s">
+      <c r="AO4" s="12" t="s">
         <v>274</v>
-      </c>
-      <c r="AN4" s="103" t="s">
-        <v>141</v>
-      </c>
-      <c r="AO4" s="103" t="s">
-        <v>141</v>
       </c>
       <c r="AP4" s="103" t="s">
         <v>141</v>
@@ -13880,26 +13959,32 @@
       <c r="AS4" s="103" t="s">
         <v>141</v>
       </c>
-      <c r="AT4" s="103" t="str">
-        <f t="shared" ref="AT4:AV5" si="0">AQ4</f>
+      <c r="AT4" s="103" t="s">
+        <v>141</v>
+      </c>
+      <c r="AU4" s="103" t="s">
+        <v>141</v>
+      </c>
+      <c r="AV4" s="103" t="str">
+        <f t="shared" ref="AV4:AX5" si="0">AS4</f>
         <v>PRC_ACTFLO</v>
       </c>
-      <c r="AU4" s="103" t="str">
+      <c r="AW4" s="103" t="str">
         <f t="shared" si="0"/>
         <v>PRC_ACTFLO</v>
       </c>
-      <c r="AV4" s="103" t="str">
+      <c r="AX4" s="103" t="str">
         <f t="shared" si="0"/>
         <v>PRC_ACTFLO</v>
       </c>
-      <c r="AW4" s="12" t="s">
+      <c r="AY4" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="AX4" s="12" t="s">
+      <c r="AZ4" s="12" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:50" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="22"/>
       <c r="H5" s="61" t="s">
         <v>27</v>
@@ -13913,12 +13998,6 @@
       <c r="O5" s="61"/>
       <c r="P5" s="61"/>
       <c r="S5" s="56"/>
-      <c r="X5" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y5" s="12" t="s">
-        <v>122</v>
-      </c>
       <c r="Z5" s="12" t="s">
         <v>122</v>
       </c>
@@ -13934,72 +14013,78 @@
       <c r="AD5" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="AE5" s="26" t="str">
+      <c r="AE5" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF5" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG5" s="26" t="str">
         <f>F14</f>
         <v>IPPPAP</v>
       </c>
-      <c r="AF5" s="12" t="str">
+      <c r="AH5" s="12" t="str">
         <f>E10</f>
         <v>IPPELC</v>
       </c>
-      <c r="AG5" s="12" t="str">
+      <c r="AI5" s="12" t="str">
         <f>E11</f>
         <v>IPPSTM</v>
       </c>
-      <c r="AH5" s="12" t="str">
+      <c r="AJ5" s="12" t="str">
         <f>E12</f>
         <v>IPPPULP</v>
       </c>
-      <c r="AI5" s="12" t="str">
+      <c r="AK5" s="12" t="str">
         <f>E15</f>
         <v>IPPREC</v>
       </c>
-      <c r="AJ5" s="12" t="str">
+      <c r="AL5" s="12" t="str">
         <f>E21</f>
         <v>IPPCOA</v>
       </c>
-      <c r="AK5" s="12" t="str">
+      <c r="AM5" s="12" t="str">
         <f>F23</f>
         <v>IPPBLQ</v>
       </c>
-      <c r="AN5" s="12" t="str">
-        <f>AF5</f>
+      <c r="AP5" s="12" t="str">
+        <f>AH5</f>
         <v>IPPELC</v>
       </c>
-      <c r="AO5" s="12" t="str">
-        <f t="shared" ref="AO5" si="1">AG5</f>
+      <c r="AQ5" s="12" t="str">
+        <f t="shared" ref="AQ5" si="1">AI5</f>
         <v>IPPSTM</v>
       </c>
-      <c r="AP5" s="12" t="str">
-        <f>AJ5</f>
+      <c r="AR5" s="12" t="str">
+        <f>AL5</f>
         <v>IPPCOA</v>
-      </c>
-      <c r="AQ5" s="12" t="str">
-        <f>AN5</f>
-        <v>IPPELC</v>
-      </c>
-      <c r="AR5" s="12" t="str">
-        <f>AO5</f>
-        <v>IPPSTM</v>
       </c>
       <c r="AS5" s="12" t="str">
         <f>AP5</f>
+        <v>IPPELC</v>
+      </c>
+      <c r="AT5" s="12" t="str">
+        <f>AQ5</f>
+        <v>IPPSTM</v>
+      </c>
+      <c r="AU5" s="12" t="str">
+        <f>AR5</f>
         <v>IPPCOA</v>
       </c>
-      <c r="AT5" s="103" t="str">
+      <c r="AV5" s="103" t="str">
         <f t="shared" si="0"/>
         <v>IPPELC</v>
       </c>
-      <c r="AU5" s="103" t="str">
+      <c r="AW5" s="103" t="str">
         <f t="shared" si="0"/>
         <v>IPPSTM</v>
       </c>
-      <c r="AV5" s="103" t="str">
+      <c r="AX5" s="103" t="str">
         <f t="shared" si="0"/>
         <v>IPPCOA</v>
       </c>
     </row>
-    <row r="6" spans="1:50" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22"/>
       <c r="H6" s="61" t="s">
         <v>122</v>
@@ -14015,9 +14100,11 @@
       <c r="U6" s="56"/>
       <c r="V6" s="56"/>
       <c r="W6" s="56"/>
-      <c r="AL6" s="53"/>
-    </row>
-    <row r="7" spans="1:50" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="X6" s="56"/>
+      <c r="Y6" s="56"/>
+      <c r="AN6" s="53"/>
+    </row>
+    <row r="7" spans="1:52" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22"/>
       <c r="B7" s="11" t="s">
         <v>56</v>
@@ -14077,35 +14164,35 @@
       <c r="W7" s="60">
         <v>2012</v>
       </c>
-      <c r="X7" s="45">
+      <c r="X7" s="60">
         <v>0</v>
       </c>
-      <c r="Y7" s="12">
-        <v>2017</v>
+      <c r="Y7" s="60">
+        <v>2012</v>
       </c>
       <c r="Z7" s="45">
         <v>0</v>
       </c>
       <c r="AA7" s="12">
+        <v>2017</v>
+      </c>
+      <c r="AB7" s="45">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="12">
         <v>2012</v>
       </c>
-      <c r="AB7" s="12">
+      <c r="AD7" s="12">
         <v>2017</v>
       </c>
-      <c r="AC7" s="12">
+      <c r="AE7" s="12">
         <v>0</v>
-      </c>
-      <c r="AD7" s="12">
-        <v>2012</v>
-      </c>
-      <c r="AE7" s="60" t="s">
-        <v>44</v>
       </c>
       <c r="AF7" s="12">
         <v>2012</v>
       </c>
-      <c r="AG7" s="12">
-        <v>2012</v>
+      <c r="AG7" s="60" t="s">
+        <v>44</v>
       </c>
       <c r="AH7" s="12">
         <v>2012</v>
@@ -14119,47 +14206,53 @@
       <c r="AK7" s="12">
         <v>2012</v>
       </c>
-      <c r="AL7" s="53" t="s">
-        <v>44</v>
+      <c r="AL7" s="12">
+        <v>2012</v>
       </c>
       <c r="AM7" s="12">
         <v>2012</v>
       </c>
-      <c r="AN7" s="12">
-        <v>2020</v>
+      <c r="AN7" s="53" t="s">
+        <v>44</v>
       </c>
       <c r="AO7" s="12">
-        <v>2020</v>
+        <v>2012</v>
       </c>
       <c r="AP7" s="12">
         <v>2020</v>
       </c>
       <c r="AQ7" s="12">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="AR7" s="12">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="AS7" s="12">
         <v>2025</v>
       </c>
       <c r="AT7" s="12">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="AU7" s="12">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="AV7" s="12">
         <v>2030</v>
       </c>
       <c r="AW7" s="12">
+        <v>2030</v>
+      </c>
+      <c r="AX7" s="12">
+        <v>2030</v>
+      </c>
+      <c r="AY7" s="12">
         <v>0</v>
       </c>
-      <c r="AX7" s="12">
+      <c r="AZ7" s="12">
         <v>2012</v>
       </c>
     </row>
-    <row r="8" spans="1:50" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:52" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>227</v>
       </c>
@@ -14180,11 +14273,13 @@
       <c r="U8" s="60"/>
       <c r="V8" s="60"/>
       <c r="W8" s="60"/>
-      <c r="X8" s="45"/>
+      <c r="X8" s="60"/>
+      <c r="Y8" s="60"/>
       <c r="Z8" s="45"/>
-      <c r="AE8" s="60"/>
-    </row>
-    <row r="9" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AB8" s="45"/>
+      <c r="AG8" s="60"/>
+    </row>
+    <row r="9" spans="1:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="57" t="str">
         <f>Processes_BASE!A8</f>
         <v>* Conversion technologies</v>
@@ -14201,7 +14296,7 @@
       <c r="N9" s="105"/>
       <c r="P9" s="105"/>
     </row>
-    <row r="10" spans="1:50" s="45" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:52" s="45" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="50" t="str">
         <f>Processes_BASE!B9</f>
@@ -14223,33 +14318,33 @@
       <c r="H10" s="105"/>
       <c r="Q10" s="102"/>
       <c r="R10" s="102"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="12"/>
       <c r="Z10" s="12"/>
       <c r="AA10" s="12"/>
       <c r="AB10" s="12"/>
       <c r="AC10" s="12"/>
       <c r="AD10" s="12"/>
-      <c r="AF10" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH(AF$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH($F$14,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="AE10" s="12"/>
+      <c r="AF10" s="12"/>
+      <c r="AH10" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH(AH$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH($F$14,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>2.5287346885513151</v>
       </c>
-      <c r="AG10" s="102"/>
-      <c r="AH10" s="129"/>
-      <c r="AN10" s="129">
-        <f>AF10</f>
+      <c r="AI10" s="102"/>
+      <c r="AJ10" s="129"/>
+      <c r="AP10" s="129">
+        <f>AH10</f>
         <v>2.5287346885513151</v>
       </c>
-      <c r="AQ10" s="45">
-        <f>AN10*(1+'PAMS levers'!$D$17)</f>
+      <c r="AS10" s="45">
+        <f>AP10*(1+'PAMS levers'!$D$17)</f>
         <v>2.2590029884391747</v>
       </c>
-      <c r="AT10" s="45">
-        <f>AN10*(1+'PAMS levers'!$E$17)</f>
+      <c r="AV10" s="45">
+        <f>AP10*(1+'PAMS levers'!$E$17)</f>
         <v>2.1241371383831047</v>
       </c>
     </row>
-    <row r="11" spans="1:50" s="45" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:52" s="45" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="E11" s="110" t="str">
         <f>RES!O2</f>
@@ -14266,33 +14361,33 @@
       <c r="P11" s="105"/>
       <c r="Q11" s="12"/>
       <c r="R11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
       <c r="Z11" s="12"/>
       <c r="AA11" s="12"/>
       <c r="AB11" s="12"/>
       <c r="AC11" s="12"/>
       <c r="AD11" s="12"/>
-      <c r="AF11" s="129"/>
-      <c r="AG11" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH(AG$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH($F$14,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="AE11" s="12"/>
+      <c r="AF11" s="12"/>
+      <c r="AH11" s="129"/>
+      <c r="AI11" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH(AI$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH($F$14,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>10.6</v>
       </c>
-      <c r="AH11" s="129"/>
-      <c r="AO11" s="129">
-        <f>AG11</f>
+      <c r="AJ11" s="129"/>
+      <c r="AQ11" s="129">
+        <f>AI11</f>
         <v>10.6</v>
       </c>
-      <c r="AR11" s="45">
-        <f>AO11*(1+'PAMS levers'!$D$17)</f>
+      <c r="AT11" s="45">
+        <f>AQ11*(1+'PAMS levers'!$D$17)</f>
         <v>9.4693333333333332</v>
       </c>
-      <c r="AU11" s="45">
-        <f>AO11*(1+'PAMS levers'!$E$17)</f>
+      <c r="AW11" s="45">
+        <f>AQ11*(1+'PAMS levers'!$E$17)</f>
         <v>8.9039999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:50" s="45" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:52" s="45" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="E12" s="109" t="str">
         <f>RES!U2</f>
@@ -14308,22 +14403,22 @@
       <c r="P12" s="105"/>
       <c r="Q12" s="12"/>
       <c r="R12" s="12"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
       <c r="AA12" s="12"/>
       <c r="AB12" s="12"/>
       <c r="AC12" s="12"/>
       <c r="AD12" s="12"/>
-      <c r="AF12" s="129"/>
-      <c r="AG12" s="129"/>
-      <c r="AH12" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH(AH$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH($F$14,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="AE12" s="12"/>
+      <c r="AF12" s="12"/>
+      <c r="AH12" s="129"/>
+      <c r="AI12" s="129"/>
+      <c r="AJ12" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH(AJ$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH($F$14,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>1.0001100887131547</v>
       </c>
-      <c r="AP12" s="129"/>
-    </row>
-    <row r="13" spans="1:50" s="45" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AR12" s="129"/>
+    </row>
+    <row r="13" spans="1:52" s="45" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="E13" s="109" t="str">
         <f>RES!E2</f>
@@ -14339,34 +14434,34 @@
       <c r="P13" s="105"/>
       <c r="Q13" s="12"/>
       <c r="R13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
       <c r="AA13" s="12"/>
       <c r="AB13" s="12"/>
       <c r="AC13" s="12"/>
       <c r="AD13" s="12"/>
-      <c r="AF13" s="129"/>
-      <c r="AG13" s="129"/>
+      <c r="AE13" s="12"/>
+      <c r="AF13" s="12"/>
       <c r="AH13" s="129"/>
-      <c r="AJ13" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH(AJ$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH($F$14,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="AI13" s="129"/>
+      <c r="AJ13" s="129"/>
+      <c r="AL13" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH(AL$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH($F$14,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>0.89999999999999991</v>
       </c>
-      <c r="AP13" s="129">
-        <f>AJ13</f>
+      <c r="AR13" s="129">
+        <f>AL13</f>
         <v>0.89999999999999991</v>
       </c>
-      <c r="AS13" s="45">
-        <f>AP13*(1+'PAMS levers'!$D$17)</f>
+      <c r="AU13" s="45">
+        <f>AR13*(1+'PAMS levers'!$D$17)</f>
         <v>0.80399999999999994</v>
       </c>
-      <c r="AV13" s="45">
-        <f>AP13*(1+'PAMS levers'!$E$17)</f>
+      <c r="AX13" s="45">
+        <f>AR13*(1+'PAMS levers'!$E$17)</f>
         <v>0.75599999999999989</v>
       </c>
     </row>
-    <row r="14" spans="1:50" s="45" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:52" s="45" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
@@ -14417,29 +14512,31 @@
         <f>SUMIFS(EB_Exist!$AF$8:$AF$12,EB_Exist!$N$8:$N$12,B10)</f>
         <v>0.85</v>
       </c>
-      <c r="V14" s="12">
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12">
         <v>3</v>
       </c>
-      <c r="W14" s="12">
+      <c r="Y14" s="12">
         <v>0</v>
       </c>
-      <c r="X14" s="12">
+      <c r="Z14" s="12">
         <v>-1</v>
       </c>
-      <c r="Y14" s="102">
+      <c r="AA14" s="102">
         <f>INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$10,EB_Exist!$N$8:$N$18,0),MATCH($F$14,EB_Exist!$R$4:$AB$4,0))</f>
         <v>2.1800600000000001</v>
       </c>
-      <c r="Z14" s="12"/>
-      <c r="AA14" s="12"/>
       <c r="AB14" s="12"/>
       <c r="AC14" s="12"/>
       <c r="AD14" s="12"/>
-      <c r="AE14" s="45">
+      <c r="AE14" s="12"/>
+      <c r="AF14" s="12"/>
+      <c r="AG14" s="45">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:50" s="45" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:52" s="45" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="50" t="str">
         <f>Processes_BASE!B10</f>
@@ -14474,21 +14571,23 @@
       <c r="V15" s="12"/>
       <c r="W15" s="12"/>
       <c r="X15" s="12"/>
-      <c r="Y15" s="102"/>
+      <c r="Y15" s="12"/>
       <c r="Z15" s="12"/>
-      <c r="AA15" s="12"/>
+      <c r="AA15" s="102"/>
       <c r="AB15" s="12"/>
       <c r="AC15" s="12"/>
       <c r="AD15" s="12"/>
-      <c r="AF15" s="129"/>
-      <c r="AG15" s="12"/>
-      <c r="AH15" s="12"/>
-      <c r="AI15" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$15,EB_Exist!$N$8:$N$18,0),MATCH(AI$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$15,EB_Exist!$N$8:$N$18,0),MATCH($F$18,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="AE15" s="12"/>
+      <c r="AF15" s="12"/>
+      <c r="AH15" s="129"/>
+      <c r="AI15" s="12"/>
+      <c r="AJ15" s="12"/>
+      <c r="AK15" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$15,EB_Exist!$N$8:$N$18,0),MATCH(AK$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$15,EB_Exist!$N$8:$N$18,0),MATCH($F$18,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>1.4893267651888342</v>
       </c>
     </row>
-    <row r="16" spans="1:50" s="45" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:52" s="45" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
@@ -14507,34 +14606,34 @@
       <c r="P16" s="12"/>
       <c r="Q16" s="12"/>
       <c r="R16" s="12"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="102"/>
       <c r="Z16" s="12"/>
-      <c r="AA16" s="12"/>
+      <c r="AA16" s="102"/>
       <c r="AB16" s="12"/>
       <c r="AC16" s="12"/>
       <c r="AD16" s="12"/>
-      <c r="AF16" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$15,EB_Exist!$N$8:$N$18,0),MATCH(AF$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$15,EB_Exist!$N$8:$N$18,0),MATCH($F$18,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="AE16" s="12"/>
+      <c r="AF16" s="12"/>
+      <c r="AH16" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$15,EB_Exist!$N$8:$N$18,0),MATCH(AH$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$15,EB_Exist!$N$8:$N$18,0),MATCH($F$18,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>0.63121997572180577</v>
       </c>
-      <c r="AG16" s="12"/>
-      <c r="AH16" s="12"/>
       <c r="AI16" s="12"/>
-      <c r="AN16" s="129">
-        <f>AF16</f>
+      <c r="AJ16" s="12"/>
+      <c r="AK16" s="12"/>
+      <c r="AP16" s="129">
+        <f>AH16</f>
         <v>0.63121997572180577</v>
       </c>
-      <c r="AQ16" s="45">
-        <f>AN16*(1+'PAMS levers'!$D$17)</f>
+      <c r="AS16" s="45">
+        <f>AP16*(1+'PAMS levers'!$D$17)</f>
         <v>0.56388984497814643</v>
       </c>
-      <c r="AT16" s="45">
-        <f>AN16*(1+'PAMS levers'!$E$17)</f>
+      <c r="AV16" s="45">
+        <f>AP16*(1+'PAMS levers'!$E$17)</f>
         <v>0.53022477960631686</v>
       </c>
     </row>
-    <row r="17" spans="1:48" s="45" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:50" s="45" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
@@ -14559,32 +14658,34 @@
       <c r="V17" s="12"/>
       <c r="W17" s="12"/>
       <c r="X17" s="12"/>
-      <c r="Y17" s="102"/>
+      <c r="Y17" s="12"/>
       <c r="Z17" s="12"/>
-      <c r="AA17" s="12"/>
+      <c r="AA17" s="102"/>
       <c r="AB17" s="12"/>
       <c r="AC17" s="12"/>
       <c r="AD17" s="12"/>
-      <c r="AG17" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$15,EB_Exist!$N$8:$N$18,0),MATCH(AG$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$15,EB_Exist!$N$8:$N$18,0),MATCH($F$18,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="AE17" s="12"/>
+      <c r="AF17" s="12"/>
+      <c r="AI17" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$15,EB_Exist!$N$8:$N$18,0),MATCH(AI$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$15,EB_Exist!$N$8:$N$18,0),MATCH($F$18,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>1.0382968436917361</v>
       </c>
-      <c r="AH17" s="12"/>
-      <c r="AI17" s="12"/>
-      <c r="AO17" s="129">
-        <f>AG17</f>
+      <c r="AJ17" s="12"/>
+      <c r="AK17" s="12"/>
+      <c r="AQ17" s="129">
+        <f>AI17</f>
         <v>1.0382968436917361</v>
       </c>
-      <c r="AR17" s="45">
-        <f>AO17*(1+'PAMS levers'!$D$17)</f>
+      <c r="AT17" s="45">
+        <f>AQ17*(1+'PAMS levers'!$D$17)</f>
         <v>0.92754518036461764</v>
       </c>
-      <c r="AU17" s="45">
-        <f>AO17*(1+'PAMS levers'!$E$17)</f>
+      <c r="AW17" s="45">
+        <f>AQ17*(1+'PAMS levers'!$E$17)</f>
         <v>0.87216934870105833</v>
       </c>
     </row>
-    <row r="18" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F18" s="110" t="str">
         <f>RES!U2</f>
         <v>IPPPULP</v>
@@ -14624,24 +14725,24 @@
         <f>SUMIFS(EB_Exist!$AF$8:$AF$12,EB_Exist!$N$8:$N$12,B15)</f>
         <v>0.85</v>
       </c>
-      <c r="V18" s="12">
+      <c r="X18" s="12">
         <v>3</v>
       </c>
-      <c r="W18" s="12">
+      <c r="Y18" s="12">
         <v>0</v>
       </c>
-      <c r="X18" s="12">
+      <c r="Z18" s="12">
         <v>-1</v>
       </c>
-      <c r="Y18" s="102">
+      <c r="AA18" s="102">
         <f>INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$15,EB_Exist!$N$8:$N$18,0),MATCH($F$18,EB_Exist!$R$4:$AB$4,0))</f>
         <v>1.218</v>
       </c>
-      <c r="AE18" s="45">
+      <c r="AG18" s="45">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="50" t="str">
         <f>Processes_BASE!B11</f>
         <v>IPPDIS-E</v>
@@ -14667,26 +14768,26 @@
       <c r="M19" s="105"/>
       <c r="N19" s="105"/>
       <c r="P19" s="111"/>
-      <c r="Y19" s="102"/>
-      <c r="AE19" s="45"/>
-      <c r="AF19" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH(AF$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH($F$22,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="AA19" s="102"/>
+      <c r="AG19" s="45"/>
+      <c r="AH19" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH(AH$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH($F$22,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>3.3106023746174635</v>
       </c>
-      <c r="AN19" s="129">
-        <f>AF19</f>
+      <c r="AP19" s="129">
+        <f>AH19</f>
         <v>3.3106023746174635</v>
       </c>
-      <c r="AQ19" s="45">
-        <f>AN19*(1+'PAMS levers'!$D$17)</f>
+      <c r="AS19" s="45">
+        <f>AP19*(1+'PAMS levers'!$D$17)</f>
         <v>2.9574714546582674</v>
       </c>
-      <c r="AT19" s="45">
-        <f>AN19*(1+'PAMS levers'!$E$17)</f>
+      <c r="AV19" s="45">
+        <f>AP19*(1+'PAMS levers'!$E$17)</f>
         <v>2.7809059946786694</v>
       </c>
     </row>
-    <row r="20" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E20" s="110" t="str">
         <f>RES!O2</f>
         <v>IPPSTM</v>
@@ -14697,51 +14798,53 @@
       <c r="U20" s="45"/>
       <c r="V20" s="45"/>
       <c r="W20" s="45"/>
-      <c r="Y20" s="102"/>
-      <c r="AE20" s="45"/>
-      <c r="AG20" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH(AG$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH($F$22,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="X20" s="45"/>
+      <c r="Y20" s="45"/>
+      <c r="AA20" s="102"/>
+      <c r="AG20" s="45"/>
+      <c r="AI20" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH(AI$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH($F$22,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>13.300000000000004</v>
       </c>
-      <c r="AO20" s="129">
-        <f>AG20</f>
+      <c r="AQ20" s="129">
+        <f>AI20</f>
         <v>13.300000000000004</v>
       </c>
-      <c r="AR20" s="45">
-        <f>AO20*(1+'PAMS levers'!$D$17)</f>
+      <c r="AT20" s="45">
+        <f>AQ20*(1+'PAMS levers'!$D$17)</f>
         <v>11.881333333333338</v>
       </c>
-      <c r="AU20" s="45">
-        <f>AO20*(1+'PAMS levers'!$E$17)</f>
+      <c r="AW20" s="45">
+        <f>AQ20*(1+'PAMS levers'!$E$17)</f>
         <v>11.172000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E21" s="110" t="str">
         <f>RES!E2</f>
         <v>IPPCOA</v>
       </c>
       <c r="F21" s="45"/>
-      <c r="Y21" s="102"/>
-      <c r="AE21" s="45"/>
-      <c r="AJ21" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH(AJ$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH($F$22,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="AA21" s="102"/>
+      <c r="AG21" s="45"/>
+      <c r="AL21" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH(AL$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH($F$22,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>3.45</v>
       </c>
-      <c r="AP21" s="129">
-        <f>AJ21</f>
+      <c r="AR21" s="129">
+        <f>AL21</f>
         <v>3.45</v>
       </c>
-      <c r="AS21" s="45">
-        <f>AP21*(1+'PAMS levers'!$D$17)</f>
+      <c r="AU21" s="45">
+        <f>AR21*(1+'PAMS levers'!$D$17)</f>
         <v>3.0820000000000003</v>
       </c>
-      <c r="AV21" s="45">
-        <f>AP21*(1+'PAMS levers'!$E$17)</f>
+      <c r="AX21" s="45">
+        <f>AR21*(1+'PAMS levers'!$E$17)</f>
         <v>2.8980000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E22" s="110"/>
       <c r="F22" s="110" t="str">
         <f>RES!AD2</f>
@@ -14785,36 +14888,36 @@
         <f>SUMIFS(EB_Exist!$AF$8:$AF$12,EB_Exist!$N$8:$N$12,B19)</f>
         <v>0.85</v>
       </c>
-      <c r="V22" s="12">
+      <c r="X22" s="12">
         <v>3</v>
       </c>
-      <c r="W22" s="12">
+      <c r="Y22" s="12">
         <v>0</v>
       </c>
-      <c r="X22" s="12">
+      <c r="Z22" s="12">
         <v>-1</v>
       </c>
-      <c r="Y22" s="102">
+      <c r="AA22" s="102">
         <f>INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH($F$22,EB_Exist!$R$4:$AB$4,0))</f>
         <v>0.65910719806663931</v>
       </c>
-      <c r="AE22" s="45">
+      <c r="AG22" s="45">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F23" s="12" t="str">
         <f>RES!V2</f>
         <v>IPPBLQ</v>
       </c>
-      <c r="Y23" s="102"/>
-      <c r="AE23" s="45"/>
-      <c r="AK23" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH(AK$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH($F$22,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="AA23" s="102"/>
+      <c r="AG23" s="45"/>
+      <c r="AM23" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH(AM$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$19,EB_Exist!$N$8:$N$18,0),MATCH($F$22,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>31.398533121995733</v>
       </c>
     </row>
-    <row r="24" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="12" t="str">
         <f>Processes_BASE!B12</f>
         <v>IPPCHE-E</v>
@@ -14831,71 +14934,71 @@
         <f>RES!D2</f>
         <v>IPPELC</v>
       </c>
-      <c r="Y24" s="102"/>
-      <c r="AF24" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH(AF$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH($F$27,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="AA24" s="102"/>
+      <c r="AH24" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH(AH$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH($F$27,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>5.4333281828562745</v>
       </c>
-      <c r="AN24" s="129">
-        <f>AF24</f>
+      <c r="AP24" s="129">
+        <f>AH24</f>
         <v>5.4333281828562745</v>
       </c>
-      <c r="AQ24" s="45">
-        <f>AN24*(1+'PAMS levers'!$D$17)</f>
+      <c r="AS24" s="45">
+        <f>AP24*(1+'PAMS levers'!$D$17)</f>
         <v>4.8537731766849381</v>
       </c>
-      <c r="AT24" s="45">
-        <f>AN24*(1+'PAMS levers'!$E$17)</f>
+      <c r="AV24" s="45">
+        <f>AP24*(1+'PAMS levers'!$E$17)</f>
         <v>4.5639956735992708</v>
       </c>
     </row>
-    <row r="25" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E25" s="12" t="str">
         <f>RES!O2</f>
         <v>IPPSTM</v>
       </c>
-      <c r="Y25" s="102"/>
-      <c r="AG25" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH(AG$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH($F$27,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="AA25" s="102"/>
+      <c r="AI25" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH(AI$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH($F$27,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>20.654552368397489</v>
       </c>
-      <c r="AO25" s="129">
-        <f>AG25</f>
+      <c r="AQ25" s="129">
+        <f>AI25</f>
         <v>20.654552368397489</v>
       </c>
-      <c r="AR25" s="45">
-        <f>AO25*(1+'PAMS levers'!$D$17)</f>
+      <c r="AT25" s="45">
+        <f>AQ25*(1+'PAMS levers'!$D$17)</f>
         <v>18.451400115768422</v>
       </c>
-      <c r="AU25" s="45">
-        <f>AO25*(1+'PAMS levers'!$E$17)</f>
+      <c r="AW25" s="45">
+        <f>AQ25*(1+'PAMS levers'!$E$17)</f>
         <v>17.349823989453892</v>
       </c>
     </row>
-    <row r="26" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E26" s="12" t="str">
         <f>RES!E2</f>
         <v>IPPCOA</v>
       </c>
-      <c r="Y26" s="102"/>
-      <c r="AJ26" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH(AJ$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH($F$27,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="AA26" s="102"/>
+      <c r="AL26" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH(AL$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH($F$27,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>5.1826921071993697</v>
       </c>
-      <c r="AP26" s="129">
-        <f>AJ26</f>
+      <c r="AR26" s="129">
+        <f>AL26</f>
         <v>5.1826921071993697</v>
       </c>
-      <c r="AS26" s="45">
-        <f>AP26*(1+'PAMS levers'!$D$17)</f>
+      <c r="AU26" s="45">
+        <f>AR26*(1+'PAMS levers'!$D$17)</f>
         <v>4.6298716157647704</v>
       </c>
-      <c r="AV26" s="45">
-        <f>AP26*(1+'PAMS levers'!$E$17)</f>
+      <c r="AX26" s="45">
+        <f>AR26*(1+'PAMS levers'!$E$17)</f>
         <v>4.3534613700474702</v>
       </c>
     </row>
-    <row r="27" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="50"/>
       <c r="F27" s="12" t="str">
         <f>RES!U2</f>
@@ -14939,35 +15042,35 @@
         <f>SUMIFS(EB_Exist!$AF$8:$AF$12,EB_Exist!$N$8:$N$12,B24)</f>
         <v>0.85</v>
       </c>
-      <c r="V27" s="12">
+      <c r="X27" s="12">
         <v>3</v>
       </c>
-      <c r="W27" s="12">
+      <c r="Y27" s="12">
         <v>0</v>
       </c>
-      <c r="X27" s="12">
+      <c r="Z27" s="12">
         <v>-1</v>
       </c>
-      <c r="Y27" s="102">
+      <c r="AA27" s="102">
         <f>INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH($F$27,EB_Exist!$R$4:$AB$4,0))</f>
         <v>0.75391051253118502</v>
       </c>
-      <c r="AE27" s="12">
+      <c r="AG27" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F28" s="12" t="str">
         <f>RES!V2</f>
         <v>IPPBLQ</v>
       </c>
-      <c r="Y28" s="102"/>
-      <c r="AK28" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH(AK$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH($F$27,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="AA28" s="102"/>
+      <c r="AM28" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH(AM$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$24,EB_Exist!$N$8:$N$18,0),MATCH($F$27,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>27.450206417681624</v>
       </c>
     </row>
-    <row r="29" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="12" t="str">
         <f>Processes_BASE!B13</f>
         <v>IPPMCH-E</v>
@@ -14984,48 +15087,48 @@
         <f>RES!D2</f>
         <v>IPPELC</v>
       </c>
-      <c r="Y29" s="102"/>
-      <c r="AF29" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$29,EB_Exist!$N$8:$N$18,0),MATCH(AF$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$29,EB_Exist!$N$8:$N$18,0),MATCH($F$31,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="AA29" s="102"/>
+      <c r="AH29" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$29,EB_Exist!$N$8:$N$18,0),MATCH(AH$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$29,EB_Exist!$N$8:$N$18,0),MATCH($F$31,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>15.941282195487931</v>
       </c>
-      <c r="AN29" s="129">
-        <f>AF29</f>
+      <c r="AP29" s="129">
+        <f>AH29</f>
         <v>15.941282195487931</v>
       </c>
-      <c r="AQ29" s="45">
-        <f>AN29*(1+'PAMS levers'!$D$17)</f>
+      <c r="AS29" s="45">
+        <f>AP29*(1+'PAMS levers'!$D$17)</f>
         <v>14.240878761302552</v>
       </c>
-      <c r="AT29" s="45">
-        <f>AN29*(1+'PAMS levers'!$E$17)</f>
+      <c r="AV29" s="45">
+        <f>AP29*(1+'PAMS levers'!$E$17)</f>
         <v>13.390677044209861</v>
       </c>
     </row>
-    <row r="30" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E30" s="12" t="str">
         <f>RES!O2</f>
         <v>IPPSTM</v>
       </c>
-      <c r="Y30" s="102"/>
-      <c r="AG30" s="129">
-        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$29,EB_Exist!$N$8:$N$18,0),MATCH(AG$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$29,EB_Exist!$N$8:$N$18,0),MATCH($F$31,EB_Exist!$R$4:$AB$4,0)))</f>
+      <c r="AA30" s="102"/>
+      <c r="AI30" s="129">
+        <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$29,EB_Exist!$N$8:$N$18,0),MATCH(AI$5,EB_Exist!$R$4:$AB$4,0))/INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$29,EB_Exist!$N$8:$N$18,0),MATCH($F$31,EB_Exist!$R$4:$AB$4,0)))</f>
         <v>7.2405257379991168</v>
       </c>
-      <c r="AO30" s="129">
-        <f>AG30</f>
+      <c r="AQ30" s="129">
+        <f>AI30</f>
         <v>7.2405257379991168</v>
       </c>
-      <c r="AR30" s="45">
-        <f>AO30*(1+'PAMS levers'!$D$17)</f>
+      <c r="AT30" s="45">
+        <f>AQ30*(1+'PAMS levers'!$D$17)</f>
         <v>6.4682029926125439</v>
       </c>
-      <c r="AU30" s="45">
-        <f>AO30*(1+'PAMS levers'!$E$17)</f>
+      <c r="AW30" s="45">
+        <f>AQ30*(1+'PAMS levers'!$E$17)</f>
         <v>6.0820416199192575</v>
       </c>
     </row>
-    <row r="31" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F31" s="12" t="str">
         <f>RES!U2</f>
         <v>IPPPULP</v>
@@ -15068,24 +15171,24 @@
         <f>SUMIFS(EB_Exist!$AF$8:$AF$12,EB_Exist!$N$8:$N$12,B29)</f>
         <v>0.85</v>
       </c>
-      <c r="V31" s="12">
+      <c r="X31" s="12">
         <v>3</v>
       </c>
-      <c r="W31" s="12">
+      <c r="Y31" s="12">
         <v>0</v>
       </c>
-      <c r="X31" s="12">
+      <c r="Z31" s="12">
         <v>-1</v>
       </c>
-      <c r="Y31" s="102">
+      <c r="AA31" s="102">
         <f>INDEX(EB_Exist!$R$8:$AB$18,MATCH($B$29,EB_Exist!$N$8:$N$18,0),MATCH($F$31,EB_Exist!$R$4:$AB$4,0))</f>
         <v>0.20838948746881503</v>
       </c>
-      <c r="AE31" s="12">
+      <c r="AG31" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="12" t="str">
         <f>Processes_BASE!B14</f>
         <v>IPPSTMCOA-E</v>
@@ -15102,36 +15205,37 @@
         <f>RES!E2</f>
         <v>IPPCOA</v>
       </c>
-      <c r="AA32" s="129">
+      <c r="AC32" s="129">
         <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B32,EB_Exist!$N$8:$N$18,0),MATCH($F33,EB_Exist!$R$4:$AB$4,0)))</f>
-        <v>40.878</v>
-      </c>
-      <c r="AB32" s="102">
-        <f>AA32</f>
-        <v>40.878</v>
-      </c>
-      <c r="AC32" s="102"/>
-      <c r="AD32" s="102"/>
-    </row>
-    <row r="33" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="AD32" s="102">
+        <f>AC32</f>
+        <v>15</v>
+      </c>
+      <c r="AE32" s="102"/>
+      <c r="AF32" s="102"/>
+    </row>
+    <row r="33" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F33" s="12" t="str">
         <f>RES!O2</f>
         <v>IPPSTM</v>
       </c>
-      <c r="H33" s="12">
-        <v>0.9</v>
+      <c r="H33" s="241">
+        <f>EB_Exist!AD14</f>
+        <v>0.33025099075297226</v>
       </c>
       <c r="I33" s="105">
         <f>SUMIFS(EB_Exist!$AC$8:$AC$17,EB_Exist!$N$8:$N$17,B32)</f>
-        <v>54.503999999999998</v>
+        <v>45.42</v>
       </c>
       <c r="J33" s="105">
         <f>I33</f>
-        <v>54.503999999999998</v>
+        <v>45.42</v>
       </c>
       <c r="K33" s="105">
         <f>J33</f>
-        <v>54.503999999999998</v>
+        <v>45.42</v>
       </c>
       <c r="M33" s="12">
         <v>0</v>
@@ -15139,17 +15243,17 @@
       <c r="S33" s="12">
         <v>1</v>
       </c>
-      <c r="V33" s="12">
+      <c r="X33" s="12">
         <v>3</v>
       </c>
-      <c r="W33" s="12">
+      <c r="Y33" s="12">
         <v>0</v>
       </c>
-      <c r="AE33" s="12">
+      <c r="AG33" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="12" t="str">
         <f>Processes_BASE!B15</f>
         <v>IPPSTMGAS-E</v>
@@ -15166,36 +15270,37 @@
         <f>RES!G2</f>
         <v>IPPGAS</v>
       </c>
-      <c r="AA34" s="129">
+      <c r="AC34" s="129">
         <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B34,EB_Exist!$N$8:$N$18,0),MATCH($F35,EB_Exist!$R$4:$AB$4,0)))</f>
-        <v>0.63971502204402642</v>
-      </c>
-      <c r="AB34" s="102">
-        <f>AA34</f>
-        <v>0.63971502204402642</v>
-      </c>
-      <c r="AC34" s="102"/>
-      <c r="AD34" s="102"/>
-    </row>
-    <row r="35" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2.4077381420440265</v>
+      </c>
+      <c r="AD34" s="102">
+        <f>AC34</f>
+        <v>2.4077381420440265</v>
+      </c>
+      <c r="AE34" s="102"/>
+      <c r="AF34" s="102"/>
+    </row>
+    <row r="35" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F35" s="12" t="str">
         <f>F33</f>
         <v>IPPSTM</v>
       </c>
-      <c r="H35" s="12">
-        <v>0.9</v>
+      <c r="H35" s="241">
+        <f>EB_Exist!AD16</f>
+        <v>0.55391979116996026</v>
       </c>
       <c r="I35" s="105">
         <f>SUMIFS(EB_Exist!$AC$8:$AC$17,EB_Exist!$N$8:$N$17,B34)</f>
-        <v>0.85295336272536848</v>
+        <v>4.3467270540352576</v>
       </c>
       <c r="J35" s="105">
         <f>I35</f>
-        <v>0.85295336272536848</v>
+        <v>4.3467270540352576</v>
       </c>
       <c r="K35" s="105">
         <f>J35</f>
-        <v>0.85295336272536848</v>
+        <v>4.3467270540352576</v>
       </c>
       <c r="M35" s="12">
         <v>0</v>
@@ -15204,16 +15309,22 @@
         <v>1</v>
       </c>
       <c r="V35" s="12">
+        <v>5</v>
+      </c>
+      <c r="W35" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="X35" s="12">
         <v>3</v>
       </c>
-      <c r="W35" s="12">
+      <c r="Y35" s="12">
         <v>0</v>
       </c>
-      <c r="AE35" s="12">
+      <c r="AG35" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="12" t="str">
         <f>Processes_BASE!B16</f>
         <v>IPPSTMBLQ-E</v>
@@ -15230,37 +15341,37 @@
         <f>RES!I2</f>
         <v>IPPBLQ</v>
       </c>
-      <c r="AA36" s="129">
+      <c r="AC36" s="129">
         <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B36,EB_Exist!$N$8:$N$18,0),MATCH($F37,EB_Exist!$R$4:$AB$4,0)))</f>
-        <v>23.313265812075059</v>
-      </c>
-      <c r="AB36" s="102">
-        <f>AA36</f>
-        <v>23.313265812075059</v>
-      </c>
-      <c r="AC36" s="102"/>
-      <c r="AD36" s="102"/>
-    </row>
-    <row r="37" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="AD36" s="102">
+        <f>AC36</f>
+        <v>25</v>
+      </c>
+      <c r="AE36" s="102"/>
+      <c r="AF36" s="102"/>
+    </row>
+    <row r="37" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F37" s="12" t="str">
         <f>F35</f>
         <v>IPPSTM</v>
       </c>
       <c r="H37" s="102">
         <f>-EB_Exist!W17/EB_Exist!U17</f>
-        <v>0.56325843742892612</v>
+        <v>0.60401065424431821</v>
       </c>
       <c r="I37" s="105">
         <f>SUMIFS(EB_Exist!$AC$8:$AC$17,EB_Exist!$N$8:$N$17,B36)</f>
-        <v>49.667998054658824</v>
+        <v>41.389998378882353</v>
       </c>
       <c r="J37" s="105">
         <f>I37</f>
-        <v>49.667998054658824</v>
+        <v>41.389998378882353</v>
       </c>
       <c r="K37" s="105">
         <f>J37</f>
-        <v>49.667998054658824</v>
+        <v>41.389998378882353</v>
       </c>
       <c r="M37" s="12">
         <v>0</v>
@@ -15268,17 +15379,17 @@
       <c r="S37" s="12">
         <v>1</v>
       </c>
-      <c r="V37" s="12">
+      <c r="X37" s="12">
         <v>3</v>
       </c>
-      <c r="W37" s="12">
+      <c r="Y37" s="12">
         <v>0</v>
       </c>
-      <c r="AE37" s="12">
+      <c r="AG37" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="12" t="str">
         <f>Processes_BASE!B17</f>
         <v>IPPSTMBIO-E</v>
@@ -15295,36 +15406,37 @@
         <f>RES!F2</f>
         <v>IPPBIO</v>
       </c>
-      <c r="AA38" s="129">
+      <c r="AC38" s="129">
         <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B38,EB_Exist!$N$8:$N$18,0),MATCH($F39,EB_Exist!$R$4:$AB$4,0)))</f>
-        <v>2.4186793036871066</v>
-      </c>
-      <c r="AB38" s="102">
-        <f>AA38</f>
-        <v>2.4186793036871066</v>
-      </c>
-      <c r="AC38" s="102"/>
-      <c r="AD38" s="102"/>
-    </row>
-    <row r="39" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AD38" s="102">
+        <f>AC38</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AE38" s="102"/>
+      <c r="AF38" s="102"/>
+    </row>
+    <row r="39" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F39" s="12" t="str">
         <f>F37</f>
         <v>IPPSTM</v>
       </c>
-      <c r="H39" s="12">
-        <v>0.9</v>
+      <c r="H39" s="241">
+        <f>EB_Exist!AD13</f>
+        <v>0.65516342057274379</v>
       </c>
       <c r="I39" s="105">
         <f>SUMIFS(EB_Exist!$AC$8:$AC$17,EB_Exist!$N$8:$N$17,B38)</f>
-        <v>3.2249057382494755</v>
+        <v>3.3579408295975384</v>
       </c>
       <c r="J39" s="105">
         <f>I39</f>
-        <v>3.2249057382494755</v>
+        <v>3.3579408295975384</v>
       </c>
       <c r="K39" s="105">
         <f>J39</f>
-        <v>3.2249057382494755</v>
+        <v>3.3579408295975384</v>
       </c>
       <c r="M39" s="12">
         <v>0</v>
@@ -15332,17 +15444,17 @@
       <c r="S39" s="12">
         <v>1</v>
       </c>
-      <c r="V39" s="12">
+      <c r="X39" s="12">
         <v>3</v>
       </c>
-      <c r="W39" s="12">
+      <c r="Y39" s="12">
         <v>0</v>
       </c>
-      <c r="AE39" s="12">
+      <c r="AG39" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="12" t="str">
         <f>Processes_BASE!B18</f>
         <v>IPPSTMCOAOIL</v>
@@ -15359,43 +15471,44 @@
         <f>RES!E2</f>
         <v>IPPCOA</v>
       </c>
-      <c r="AA40" s="129">
+      <c r="AC40" s="129">
         <f>ABS(INDEX(EB_Exist!$R$8:$AB$18,MATCH($B40,EB_Exist!$N$8:$N$18,0),MATCH($F42,EB_Exist!$R$4:$AB$4,0)))</f>
-        <v>8.6685828765799702</v>
-      </c>
-      <c r="AB40" s="102">
-        <f>AA40</f>
-        <v>8.6685828765799702</v>
-      </c>
-      <c r="AC40" s="102"/>
-      <c r="AD40" s="102"/>
-      <c r="AJ40" s="129"/>
-    </row>
-    <row r="41" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="AD40" s="102">
+        <f>AC40</f>
+        <v>6</v>
+      </c>
+      <c r="AE40" s="102"/>
+      <c r="AF40" s="102"/>
+      <c r="AL40" s="129"/>
+    </row>
+    <row r="41" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E41" s="12" t="str">
         <f>RES!H2</f>
         <v>IPPOHF</v>
       </c>
     </row>
-    <row r="42" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F42" s="12" t="str">
         <f>F39</f>
         <v>IPPSTM</v>
       </c>
-      <c r="H42" s="12">
-        <v>0.9</v>
+      <c r="H42" s="241">
+        <f>EB_Exist!AD15</f>
+        <v>0.48196222627019669</v>
       </c>
       <c r="I42" s="105">
         <f>SUMIFS(EB_Exist!$AC$8:$AC$17,EB_Exist!$N$8:$N$17,B40)</f>
-        <v>11.558110502106626</v>
+        <v>12.449108400948194</v>
       </c>
       <c r="J42" s="105">
         <f>I42</f>
-        <v>11.558110502106626</v>
+        <v>12.449108400948194</v>
       </c>
       <c r="K42" s="105">
         <f>J42</f>
-        <v>11.558110502106626</v>
+        <v>12.449108400948194</v>
       </c>
       <c r="M42" s="12">
         <v>0</v>
@@ -15403,17 +15516,17 @@
       <c r="S42" s="12">
         <v>1</v>
       </c>
-      <c r="V42" s="12">
+      <c r="X42" s="12">
         <v>3</v>
       </c>
-      <c r="W42" s="12">
+      <c r="Y42" s="12">
         <v>0</v>
       </c>
-      <c r="AE42" s="12">
+      <c r="AG42" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="12" t="str">
         <f>Processes_BASE!B19</f>
         <v>IPPELCSTM-E</v>
@@ -15430,9 +15543,9 @@
         <f>RES!O2</f>
         <v>IPPSTM</v>
       </c>
-      <c r="AA43" s="129"/>
-    </row>
-    <row r="44" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AC43" s="129"/>
+    </row>
+    <row r="44" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F44" s="12" t="str">
         <f>RES!D2</f>
         <v>IPPELC</v>
@@ -15458,14 +15571,14 @@
       <c r="S44" s="12">
         <v>1</v>
       </c>
-      <c r="V44" s="12">
+      <c r="X44" s="12">
         <v>3</v>
       </c>
-      <c r="W44" s="12">
+      <c r="Y44" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="12" t="str">
         <f>Processes_BASE!B20</f>
         <v>IPPPAP-E-T1</v>
@@ -15500,21 +15613,21 @@
       <c r="U45" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE45" s="12">
+      <c r="AG45" s="12">
         <v>1</v>
       </c>
-      <c r="AH45" s="102">
-        <f>AH12</f>
+      <c r="AJ45" s="102">
+        <f>AJ12</f>
         <v>1.0001100887131547</v>
       </c>
-      <c r="AW45" s="12">
+      <c r="AY45" s="12">
         <v>5</v>
       </c>
-      <c r="AX45" s="12">
+      <c r="AZ45" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="12" t="str">
         <f>Processes_BASE!B21</f>
         <v>IPPREC-E-T1</v>
@@ -15549,21 +15662,21 @@
       <c r="U46" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE46" s="12">
+      <c r="AG46" s="12">
         <v>1</v>
       </c>
-      <c r="AI46" s="102">
-        <f>AI15</f>
+      <c r="AK46" s="102">
+        <f>AK15</f>
         <v>1.4893267651888342</v>
       </c>
-      <c r="AW46" s="12">
+      <c r="AY46" s="12">
         <v>5</v>
       </c>
-      <c r="AX46" s="12">
+      <c r="AZ46" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="12" t="str">
         <f>Processes_BASE!B22</f>
         <v>IPPDIS-E-T1</v>
@@ -15598,21 +15711,21 @@
       <c r="U47" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE47" s="12">
+      <c r="AG47" s="12">
         <v>1</v>
       </c>
-      <c r="AK47" s="102">
-        <f>AK23</f>
+      <c r="AM47" s="102">
+        <f>AM23</f>
         <v>31.398533121995733</v>
       </c>
-      <c r="AW47" s="12">
+      <c r="AY47" s="12">
         <v>5</v>
       </c>
-      <c r="AX47" s="12">
+      <c r="AZ47" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F48" s="12" t="str">
         <f>F23</f>
         <v>IPPBLQ</v>
@@ -15625,7 +15738,7 @@
       </c>
       <c r="R48" s="190"/>
     </row>
-    <row r="49" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="12" t="str">
         <f>Processes_BASE!B23</f>
         <v>IPPCHE-E-T1</v>
@@ -15660,21 +15773,21 @@
       <c r="U49" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE49" s="12">
+      <c r="AG49" s="12">
         <v>1</v>
       </c>
-      <c r="AK49" s="102">
-        <f>AK28</f>
+      <c r="AM49" s="102">
+        <f>AM28</f>
         <v>27.450206417681624</v>
       </c>
-      <c r="AW49" s="12">
+      <c r="AY49" s="12">
         <v>5</v>
       </c>
-      <c r="AX49" s="12">
+      <c r="AZ49" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F50" s="12" t="str">
         <f>F28</f>
         <v>IPPBLQ</v>
@@ -15687,7 +15800,7 @@
       </c>
       <c r="R50" s="190"/>
     </row>
-    <row r="51" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="12" t="str">
         <f>Processes_BASE!B24</f>
         <v>IPPMCH-E-T1</v>
@@ -15722,17 +15835,17 @@
       <c r="U51" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE51" s="12">
+      <c r="AG51" s="12">
         <v>1</v>
       </c>
-      <c r="AW51" s="12">
+      <c r="AY51" s="12">
         <v>5</v>
       </c>
-      <c r="AX51" s="12">
+      <c r="AZ51" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="12" t="str">
         <f>Processes_BASE!B25</f>
         <v>IPPPAP-E-T2</v>
@@ -15767,21 +15880,21 @@
       <c r="U52" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE52" s="12">
+      <c r="AG52" s="12">
         <v>1</v>
       </c>
-      <c r="AH52" s="102">
-        <f>AH45</f>
+      <c r="AJ52" s="102">
+        <f>AJ45</f>
         <v>1.0001100887131547</v>
       </c>
-      <c r="AW52" s="12">
+      <c r="AY52" s="12">
         <v>5</v>
       </c>
-      <c r="AX52" s="12">
+      <c r="AZ52" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="12" t="str">
         <f>Processes_BASE!B26</f>
         <v>IPPREC-E-T2</v>
@@ -15816,21 +15929,21 @@
       <c r="U53" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE53" s="12">
+      <c r="AG53" s="12">
         <v>1</v>
       </c>
-      <c r="AI53" s="102">
-        <f>AI46</f>
+      <c r="AK53" s="102">
+        <f>AK46</f>
         <v>1.4893267651888342</v>
       </c>
-      <c r="AW53" s="12">
+      <c r="AY53" s="12">
         <v>5</v>
       </c>
-      <c r="AX53" s="12">
+      <c r="AZ53" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="12" t="str">
         <f>Processes_BASE!B27</f>
         <v>IPPDIS-E-T2</v>
@@ -15865,21 +15978,21 @@
       <c r="U54" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE54" s="12">
+      <c r="AG54" s="12">
         <v>1</v>
       </c>
-      <c r="AK54" s="102">
-        <f>AK47</f>
+      <c r="AM54" s="102">
+        <f>AM47</f>
         <v>31.398533121995733</v>
       </c>
-      <c r="AW54" s="12">
+      <c r="AY54" s="12">
         <v>5</v>
       </c>
-      <c r="AX54" s="12">
+      <c r="AZ54" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F55" s="12" t="str">
         <f t="shared" si="2"/>
         <v>IPPBLQ</v>
@@ -15892,7 +16005,7 @@
       </c>
       <c r="R55" s="190"/>
     </row>
-    <row r="56" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="12" t="str">
         <f>Processes_BASE!B28</f>
         <v>IPPCHE-E-T2</v>
@@ -15927,21 +16040,21 @@
       <c r="U56" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE56" s="12">
+      <c r="AG56" s="12">
         <v>1</v>
       </c>
-      <c r="AK56" s="102">
-        <f>AK49</f>
+      <c r="AM56" s="102">
+        <f>AM49</f>
         <v>27.450206417681624</v>
       </c>
-      <c r="AW56" s="12">
+      <c r="AY56" s="12">
         <v>5</v>
       </c>
-      <c r="AX56" s="12">
+      <c r="AZ56" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F57" s="12" t="str">
         <f t="shared" si="2"/>
         <v>IPPBLQ</v>
@@ -15954,7 +16067,7 @@
       </c>
       <c r="R57" s="190"/>
     </row>
-    <row r="58" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="12" t="str">
         <f>Processes_BASE!B29</f>
         <v>IPPMCH-E-T2</v>
@@ -15989,17 +16102,17 @@
       <c r="U58" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE58" s="12">
+      <c r="AG58" s="12">
         <v>1</v>
       </c>
-      <c r="AW58" s="12">
+      <c r="AY58" s="12">
         <v>5</v>
       </c>
-      <c r="AX58" s="12">
+      <c r="AZ58" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="12" t="str">
         <f>Processes_BASE!B30</f>
         <v>IPPPAP-N</v>
@@ -16016,42 +16129,42 @@
         <f>E10</f>
         <v>IPPELC</v>
       </c>
-      <c r="AF59" s="102">
-        <f>AF10</f>
+      <c r="AH59" s="102">
+        <f>AH10</f>
         <v>2.5287346885513151</v>
       </c>
     </row>
-    <row r="60" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E60" s="12" t="str">
         <f t="shared" ref="E60:F63" si="3">E11</f>
         <v>IPPSTM</v>
       </c>
-      <c r="AG60" s="102">
-        <f>AG11</f>
+      <c r="AI60" s="102">
+        <f>AI11</f>
         <v>10.6</v>
       </c>
     </row>
-    <row r="61" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E61" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IPPPULP</v>
       </c>
-      <c r="AH61" s="102">
-        <f>AH12</f>
+      <c r="AJ61" s="102">
+        <f>AJ12</f>
         <v>1.0001100887131547</v>
       </c>
     </row>
-    <row r="62" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E62" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IPPCOA</v>
       </c>
-      <c r="AJ62" s="102">
-        <f>AJ13</f>
+      <c r="AL62" s="102">
+        <f>AL13</f>
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="63" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F63" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IPPPAP</v>
@@ -16072,18 +16185,18 @@
       <c r="U63" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE63" s="12">
+      <c r="AG63" s="12">
         <v>1</v>
       </c>
-      <c r="AI63" s="102"/>
-      <c r="AL63" s="12">
+      <c r="AK63" s="102"/>
+      <c r="AN63" s="12">
         <v>2025</v>
       </c>
-      <c r="AM63" s="12">
+      <c r="AO63" s="12">
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="2:50" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="12" t="str">
         <f>Processes_BASE!B31</f>
         <v>IPPREC-N</v>
@@ -16100,32 +16213,32 @@
         <f>E15</f>
         <v>IPPREC</v>
       </c>
-      <c r="AI64" s="102">
-        <f>AI15</f>
+      <c r="AK64" s="102">
+        <f>AK15</f>
         <v>1.4893267651888342</v>
       </c>
     </row>
-    <row r="65" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E65" s="12" t="str">
         <f t="shared" ref="E65:F67" si="4">E16</f>
         <v>IPPELC</v>
       </c>
-      <c r="AF65" s="102">
-        <f>AF16</f>
+      <c r="AH65" s="102">
+        <f>AH16</f>
         <v>0.63121997572180577</v>
       </c>
     </row>
-    <row r="66" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E66" s="12" t="str">
         <f t="shared" si="4"/>
         <v>IPPSTM</v>
       </c>
-      <c r="AG66" s="102">
-        <f>AG17</f>
+      <c r="AI66" s="102">
+        <f>AI17</f>
         <v>1.0382968436917361</v>
       </c>
     </row>
-    <row r="67" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F67" s="12" t="str">
         <f t="shared" si="4"/>
         <v>IPPPULP</v>
@@ -16146,17 +16259,17 @@
       <c r="U67" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE67" s="12">
+      <c r="AG67" s="12">
         <v>1</v>
       </c>
-      <c r="AL67" s="12">
+      <c r="AN67" s="12">
         <v>2025</v>
       </c>
-      <c r="AM67" s="12">
+      <c r="AO67" s="12">
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="12" t="str">
         <f>Processes_BASE!B32</f>
         <v>IPPDIS-N</v>
@@ -16173,36 +16286,36 @@
         <f>E19</f>
         <v>IPPELC</v>
       </c>
-      <c r="AF68" s="102">
-        <f>AF19</f>
+      <c r="AH68" s="102">
+        <f>AH19</f>
         <v>3.3106023746174635</v>
       </c>
-      <c r="AG68" s="102"/>
-    </row>
-    <row r="69" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AI68" s="102"/>
+    </row>
+    <row r="69" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E69" s="12" t="str">
         <f t="shared" ref="E69:F72" si="5">E20</f>
         <v>IPPSTM</v>
       </c>
-      <c r="AF69" s="102"/>
-      <c r="AG69" s="102">
-        <f t="shared" ref="AG69" si="6">AG20</f>
+      <c r="AH69" s="102"/>
+      <c r="AI69" s="102">
+        <f t="shared" ref="AI69" si="6">AI20</f>
         <v>13.300000000000004</v>
       </c>
     </row>
-    <row r="70" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E70" s="12" t="str">
         <f t="shared" si="5"/>
         <v>IPPCOA</v>
       </c>
-      <c r="AF70" s="102"/>
-      <c r="AG70" s="102"/>
-      <c r="AJ70" s="176">
-        <f>AJ26</f>
+      <c r="AH70" s="102"/>
+      <c r="AI70" s="102"/>
+      <c r="AL70" s="176">
+        <f>AL26</f>
         <v>5.1826921071993697</v>
       </c>
     </row>
-    <row r="71" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F71" s="12" t="str">
         <f t="shared" si="5"/>
         <v>IPPPULPD</v>
@@ -16223,27 +16336,27 @@
       <c r="U71" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE71" s="12">
+      <c r="AG71" s="12">
         <v>1</v>
       </c>
-      <c r="AL71" s="12">
+      <c r="AN71" s="12">
         <v>2025</v>
       </c>
-      <c r="AM71" s="12">
+      <c r="AO71" s="12">
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F72" s="12" t="str">
         <f t="shared" si="5"/>
         <v>IPPBLQ</v>
       </c>
-      <c r="AK72" s="102">
-        <f>AK23</f>
+      <c r="AM72" s="102">
+        <f>AM23</f>
         <v>31.398533121995733</v>
       </c>
     </row>
-    <row r="73" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="12" t="str">
         <f>Processes_BASE!B33</f>
         <v>IPPCHE-N</v>
@@ -16260,32 +16373,32 @@
         <f>E24</f>
         <v>IPPELC</v>
       </c>
-      <c r="AF73" s="102">
-        <f>AF24</f>
+      <c r="AH73" s="102">
+        <f>AH24</f>
         <v>5.4333281828562745</v>
       </c>
     </row>
-    <row r="74" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E74" s="12" t="str">
         <f t="shared" ref="E74:E75" si="7">E25</f>
         <v>IPPSTM</v>
       </c>
-      <c r="AG74" s="102">
-        <f>AG25</f>
+      <c r="AI74" s="102">
+        <f>AI25</f>
         <v>20.654552368397489</v>
       </c>
     </row>
-    <row r="75" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E75" s="12" t="str">
         <f t="shared" si="7"/>
         <v>IPPCOA</v>
       </c>
-      <c r="AJ75" s="102">
-        <f>AJ26</f>
+      <c r="AL75" s="102">
+        <f>AL26</f>
         <v>5.1826921071993697</v>
       </c>
     </row>
-    <row r="76" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F76" s="12" t="str">
         <f>F27</f>
         <v>IPPPULP</v>
@@ -16306,27 +16419,27 @@
       <c r="U76" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE76" s="12">
+      <c r="AG76" s="12">
         <v>1</v>
       </c>
-      <c r="AL76" s="12">
+      <c r="AN76" s="12">
         <v>2025</v>
       </c>
-      <c r="AM76" s="12">
+      <c r="AO76" s="12">
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F77" s="12" t="str">
         <f>F28</f>
         <v>IPPBLQ</v>
       </c>
-      <c r="AK77" s="102">
-        <f>AK28</f>
+      <c r="AM77" s="102">
+        <f>AM28</f>
         <v>27.450206417681624</v>
       </c>
     </row>
-    <row r="78" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="12" t="str">
         <f>Processes_BASE!B34</f>
         <v>IPPMCH-N</v>
@@ -16343,22 +16456,22 @@
         <f>E29</f>
         <v>IPPELC</v>
       </c>
-      <c r="AF78" s="102">
-        <f>AF29</f>
+      <c r="AH78" s="102">
+        <f>AH29</f>
         <v>15.941282195487931</v>
       </c>
     </row>
-    <row r="79" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E79" s="12" t="str">
         <f>E30</f>
         <v>IPPSTM</v>
       </c>
-      <c r="AG79" s="102">
-        <f>AG30</f>
+      <c r="AI79" s="102">
+        <f>AI30</f>
         <v>7.2405257379991168</v>
       </c>
     </row>
-    <row r="80" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F80" s="12" t="str">
         <f>F31</f>
         <v>IPPPULP</v>
@@ -16379,17 +16492,17 @@
       <c r="U80" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE80" s="12">
+      <c r="AG80" s="12">
         <v>1</v>
       </c>
-      <c r="AL80" s="12">
+      <c r="AN80" s="12">
         <v>2025</v>
       </c>
-      <c r="AM80" s="12">
+      <c r="AO80" s="12">
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="12" t="str">
         <f>Processes_BASE!B35</f>
         <v>IPPSTMCOA-N</v>
@@ -16407,14 +16520,14 @@
         <v>IPPCOA</v>
       </c>
     </row>
-    <row r="82" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F82" s="12" t="str">
         <f>F33</f>
         <v>IPPSTM</v>
       </c>
       <c r="H82" s="12">
         <f>H33</f>
-        <v>0.9</v>
+        <v>0.33025099075297226</v>
       </c>
       <c r="I82" s="12">
         <v>0</v>
@@ -16432,17 +16545,17 @@
       <c r="U82" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE82" s="12">
+      <c r="AG82" s="12">
         <v>1</v>
       </c>
-      <c r="AL82" s="196">
+      <c r="AN82" s="196">
         <v>2031</v>
       </c>
-      <c r="AM82" s="12">
+      <c r="AO82" s="12">
         <v>40</v>
       </c>
     </row>
-    <row r="83" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="12" t="str">
         <f>Processes_BASE!B36</f>
         <v>IPPSTMGAS-N</v>
@@ -16456,14 +16569,14 @@
         <v>IPPGAS</v>
       </c>
     </row>
-    <row r="84" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F84" s="12" t="str">
         <f>F35</f>
         <v>IPPSTM</v>
       </c>
       <c r="H84" s="12">
         <f>H35</f>
-        <v>0.9</v>
+        <v>0.55391979116996026</v>
       </c>
       <c r="I84" s="12">
         <v>0</v>
@@ -16481,17 +16594,17 @@
       <c r="U84" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE84" s="12">
+      <c r="AG84" s="12">
         <v>1</v>
       </c>
-      <c r="AL84" s="196">
+      <c r="AN84" s="196">
         <v>2031</v>
       </c>
-      <c r="AM84" s="12">
+      <c r="AO84" s="12">
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B85" s="12" t="str">
         <f>Processes_BASE!B37</f>
         <v>IPPSTMBLQ-N</v>
@@ -16505,14 +16618,14 @@
         <v>IPPBLQ</v>
       </c>
     </row>
-    <row r="86" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F86" s="12" t="str">
         <f>F37</f>
         <v>IPPSTM</v>
       </c>
       <c r="H86" s="12">
         <f>H37</f>
-        <v>0.56325843742892612</v>
+        <v>0.60401065424431821</v>
       </c>
       <c r="I86" s="12">
         <v>0</v>
@@ -16530,17 +16643,17 @@
       <c r="U86" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE86" s="12">
+      <c r="AG86" s="12">
         <v>1</v>
       </c>
-      <c r="AL86" s="196">
+      <c r="AN86" s="196">
         <v>2031</v>
       </c>
-      <c r="AM86" s="12">
+      <c r="AO86" s="12">
         <v>40</v>
       </c>
     </row>
-    <row r="87" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="12" t="str">
         <f>Processes_BASE!B38</f>
         <v>IPPSTMBIO-N</v>
@@ -16554,14 +16667,14 @@
         <v>IPPBIO</v>
       </c>
     </row>
-    <row r="88" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F88" s="12" t="str">
         <f>F39</f>
         <v>IPPSTM</v>
       </c>
       <c r="H88" s="12">
         <f>H39</f>
-        <v>0.9</v>
+        <v>0.65516342057274379</v>
       </c>
       <c r="I88" s="12">
         <v>0</v>
@@ -16579,17 +16692,17 @@
       <c r="U88" s="12">
         <v>0.85</v>
       </c>
-      <c r="AE88" s="12">
+      <c r="AG88" s="12">
         <v>1</v>
       </c>
-      <c r="AL88" s="196">
+      <c r="AN88" s="196">
         <v>2031</v>
       </c>
-      <c r="AM88" s="12">
+      <c r="AO88" s="12">
         <v>40</v>
       </c>
     </row>
-    <row r="89" spans="2:39" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:41" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B89" s="12" t="str">
         <f>Processes_BASE!B46</f>
         <v>XIPPREC</v>
@@ -16606,10 +16719,10 @@
         <f>RES!J2</f>
         <v>IPPREC</v>
       </c>
-      <c r="AC89" s="12">
+      <c r="AE89" s="12">
         <v>5</v>
       </c>
-      <c r="AD89" s="12">
+      <c r="AF89" s="12">
         <f>'PAMS levers'!E22</f>
         <v>2.7210000000000001</v>
       </c>
@@ -16634,7 +16747,7 @@
               </from>
               <to>
                 <xdr:col>2</xdr:col>
-                <xdr:colOff>857250</xdr:colOff>
+                <xdr:colOff>847725</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -16810,6 +16923,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="K39" sqref="K39"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17638,6 +17752,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17736,6 +17851,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17808,9 +17924,9 @@
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>247650</xdr:colOff>
+                <xdr:colOff>238125</xdr:colOff>
                 <xdr:row>12</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -17833,9 +17949,9 @@
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
+                <xdr:colOff>228600</xdr:colOff>
                 <xdr:row>28</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -17858,9 +17974,9 @@
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>247650</xdr:colOff>
+                <xdr:colOff>238125</xdr:colOff>
                 <xdr:row>6</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -17883,9 +17999,9 @@
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>590550</xdr:colOff>
+                <xdr:colOff>571500</xdr:colOff>
                 <xdr:row>17</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -17908,9 +18024,9 @@
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>561975</xdr:colOff>
-                <xdr:row>22</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:colOff>552450</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -17934,6 +18050,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18660,7 +18777,7 @@
               </from>
               <to>
                 <xdr:col>2</xdr:col>
-                <xdr:colOff>847725</xdr:colOff>
+                <xdr:colOff>838200</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>228600</xdr:rowOff>
               </to>
@@ -18762,7 +18879,7 @@
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>819150</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -18833,6 +18950,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="K33" sqref="K33"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19065,6 +19183,7 @@
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19518,7 +19637,7 @@
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>819150</xdr:colOff>
                 <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>28575</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -19541,7 +19660,7 @@
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>238125</xdr:rowOff>
               </to>
@@ -19566,7 +19685,7 @@
               </from>
               <to>
                 <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>238125</xdr:rowOff>
               </to>
@@ -19613,6 +19732,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19835,7 +19955,7 @@
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>95250</xdr:rowOff>
               </to>
@@ -19857,6 +19977,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19931,7 +20052,7 @@
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>819150</xdr:colOff>
                 <xdr:row>6</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -20176,6 +20297,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20435,6 +20557,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20508,9 +20631,9 @@
               </from>
               <to>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>857250</xdr:colOff>
+                <xdr:colOff>847725</xdr:colOff>
                 <xdr:row>6</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -20755,6 +20878,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20839,10 +20963,10 @@
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>838200</xdr:colOff>
                 <xdr:row>5</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -21064,8 +21188,8 @@
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>838200</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -21087,6 +21211,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -21359,6 +21484,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -21445,7 +21571,7 @@
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>666750</xdr:colOff>
                 <xdr:row>6</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -21668,7 +21794,7 @@
               </from>
               <to>
                 <xdr:col>10</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>85725</xdr:rowOff>
               </to>
@@ -21694,6 +21820,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -21845,9 +21972,10 @@
   </sheetPr>
   <dimension ref="B2:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -22038,9 +22166,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C6D8D9-7BAD-4B1A-A6EC-C2F84D7DAE50}">
   <dimension ref="B2:N107"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L105" sqref="L105"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -23838,9 +23967,10 @@
   </sheetPr>
   <dimension ref="B1:AJ105"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26997,7 +27127,10 @@
   <dimension ref="A1:AF74"/>
   <sheetViews>
     <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27"/>
+      <selection activeCell="AD16" sqref="AD16"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="1">
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -27034,7 +27167,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="97"/>
       <c r="B2" s="92"/>
       <c r="C2" s="113" t="s">
@@ -27049,6 +27182,14 @@
       <c r="J2" s="92"/>
       <c r="K2" s="92"/>
       <c r="L2" s="93"/>
+      <c r="R2" s="235" t="s">
+        <v>347</v>
+      </c>
+      <c r="S2" s="235"/>
+      <c r="T2" s="235"/>
+      <c r="U2" s="235"/>
+      <c r="V2" s="235"/>
+      <c r="W2" s="235"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="98" t="s">
@@ -27705,21 +27846,22 @@
       <c r="V13" s="165">
         <v>0</v>
       </c>
-      <c r="W13" s="165">
-        <v>2.4186793036871066</v>
+      <c r="W13" s="236">
+        <v>2.2000000000000002</v>
       </c>
       <c r="X13" s="168">
         <v>0</v>
       </c>
       <c r="AC13" s="183">
         <f>(W13/AD13)*AE13</f>
-        <v>3.2249057382494755</v>
-      </c>
-      <c r="AD13">
-        <v>0.9</v>
+        <v>3.3579408295975384</v>
+      </c>
+      <c r="AD13" s="226">
+        <f>-W13/SUM(R13:V13)</f>
+        <v>0.65516342057274379</v>
       </c>
       <c r="AE13" s="179">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:32" ht="15" x14ac:dyDescent="0.25">
@@ -27763,22 +27905,22 @@
       <c r="V14" s="163">
         <v>0</v>
       </c>
-      <c r="W14" s="180">
-        <f>-R14*AD14</f>
-        <v>40.878</v>
+      <c r="W14" s="237">
+        <v>15</v>
       </c>
       <c r="X14" s="169">
         <v>0</v>
       </c>
       <c r="AC14" s="183">
         <f>(W14/AD14)*AE14</f>
-        <v>54.503999999999998</v>
-      </c>
-      <c r="AD14">
-        <v>0.9</v>
+        <v>45.42</v>
+      </c>
+      <c r="AD14" s="226">
+        <f>-W14/SUM(R14:V14)</f>
+        <v>0.33025099075297226</v>
       </c>
       <c r="AE14" s="179">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.2">
@@ -27823,21 +27965,22 @@
       <c r="V15" s="163">
         <v>-0.43865303346417234</v>
       </c>
-      <c r="W15" s="163">
-        <v>8.6685828765799702</v>
+      <c r="W15" s="237">
+        <v>6</v>
       </c>
       <c r="X15" s="169">
         <v>0</v>
       </c>
       <c r="AC15" s="183">
         <f>(W15/AD15)*AE15</f>
-        <v>11.558110502106626</v>
-      </c>
-      <c r="AD15">
-        <v>0.9</v>
+        <v>12.449108400948194</v>
+      </c>
+      <c r="AD15" s="226">
+        <f>-W15/SUM(R15:V15)</f>
+        <v>0.48196222627019669</v>
       </c>
       <c r="AE15" s="179">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.2">
@@ -27866,7 +28009,7 @@
         <v>0</v>
       </c>
       <c r="T16" s="163">
-        <v>-2.0194860031331041</v>
+        <v>-4.3467270540352576</v>
       </c>
       <c r="U16" s="163">
         <v>0</v>
@@ -27874,21 +28017,22 @@
       <c r="V16" s="163">
         <v>0</v>
       </c>
-      <c r="W16" s="163">
-        <v>0.63971502204402642</v>
+      <c r="W16" s="237">
+        <v>2.4077381420440265</v>
       </c>
       <c r="X16" s="169">
         <v>0</v>
       </c>
       <c r="AC16" s="183">
         <f>(W16/AD16)*AE16</f>
-        <v>0.85295336272536848</v>
-      </c>
-      <c r="AD16">
-        <v>0.9</v>
+        <v>4.3467270540352576</v>
+      </c>
+      <c r="AD16" s="226">
+        <f t="shared" ref="AD16:AD17" si="0">-W16/SUM(R16:V16)</f>
+        <v>0.55391979116996026</v>
       </c>
       <c r="AE16" s="179">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
@@ -27926,22 +28070,22 @@
       <c r="V17" s="164">
         <v>0</v>
       </c>
-      <c r="W17" s="164">
-        <v>23.313265812075059</v>
+      <c r="W17" s="238">
+        <v>25</v>
       </c>
       <c r="X17" s="170">
         <v>0</v>
       </c>
       <c r="AC17" s="183">
         <f>(W17/AD17)*AE17</f>
-        <v>49.667998054658824</v>
-      </c>
-      <c r="AD17" s="182">
-        <f>-W17/U17</f>
-        <v>0.56325843742892612</v>
+        <v>41.389998378882353</v>
+      </c>
+      <c r="AD17" s="226">
+        <f t="shared" si="0"/>
+        <v>0.60401065424431821</v>
       </c>
       <c r="AE17" s="179">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -27977,9 +28121,7 @@
       <c r="V18" s="166">
         <v>-0.43865303346417234</v>
       </c>
-      <c r="W18" s="166">
-        <v>61.552020097249219</v>
-      </c>
+      <c r="W18" s="166"/>
       <c r="X18" s="171">
         <v>0</v>
       </c>
@@ -28174,6 +28316,13 @@
       <c r="S25" s="84"/>
       <c r="T25" s="84"/>
       <c r="U25" s="84"/>
+      <c r="V25" s="163">
+        <f>SUM(W13:W17)</f>
+        <v>50.607738142044028</v>
+      </c>
+      <c r="W25" s="84" t="s">
+        <v>348</v>
+      </c>
       <c r="Y25" s="223">
         <f>Y24+Y23</f>
         <v>2180300</v>
@@ -28196,6 +28345,13 @@
       <c r="K26" s="91"/>
       <c r="L26" s="90"/>
       <c r="Q26" s="84"/>
+      <c r="V26" s="163">
+        <f>SUM(W8:W12)</f>
+        <v>-50.219940899609995</v>
+      </c>
+      <c r="W26" s="84" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="90"/>
@@ -28211,6 +28367,10 @@
       <c r="K27" s="90"/>
       <c r="L27" s="90"/>
       <c r="Q27" s="84"/>
+      <c r="V27" s="163">
+        <f>SUM(V25:V26)</f>
+        <v>0.3877972424340328</v>
+      </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" s="90"/>
@@ -28256,6 +28416,9 @@
       <c r="J30" s="90"/>
       <c r="K30" s="90"/>
       <c r="L30" s="90"/>
+      <c r="W30" s="239" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" s="90"/>
@@ -28271,6 +28434,7 @@
       <c r="K31" s="90"/>
       <c r="L31" s="90"/>
       <c r="M31" s="84"/>
+      <c r="W31" s="240"/>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" s="90"/>
@@ -28285,8 +28449,9 @@
       <c r="J32" s="90"/>
       <c r="K32" s="90"/>
       <c r="L32" s="90"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="W32" s="240"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" s="90"/>
       <c r="B33" s="155"/>
       <c r="C33" s="90"/>
@@ -28300,8 +28465,9 @@
       <c r="K33" s="90"/>
       <c r="L33" s="90"/>
       <c r="M33" s="84"/>
-    </row>
-    <row r="34" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W33" s="240"/>
+    </row>
+    <row r="34" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="90"/>
       <c r="B34" s="155"/>
       <c r="C34" s="90"/>
@@ -28315,8 +28481,9 @@
       <c r="K34" s="90"/>
       <c r="L34" s="90"/>
       <c r="M34" s="84"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="W34" s="240"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="90"/>
       <c r="B35" s="155"/>
       <c r="C35" s="90"/>
@@ -28331,7 +28498,7 @@
       <c r="L35" s="90"/>
       <c r="M35" s="84"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" s="90"/>
       <c r="B36" s="155"/>
       <c r="C36" s="90"/>
@@ -28346,7 +28513,7 @@
       <c r="L36" s="90"/>
       <c r="M36" s="84"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" s="90"/>
       <c r="B37" s="155"/>
       <c r="C37" s="90"/>
@@ -28361,7 +28528,7 @@
       <c r="L37" s="90"/>
       <c r="M37" s="84"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" s="90"/>
       <c r="B38" s="155"/>
       <c r="C38" s="90"/>
@@ -28376,40 +28543,40 @@
       <c r="L38" s="90"/>
       <c r="M38" s="84"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" s="90"/>
       <c r="B39" s="155"/>
       <c r="M39" s="84"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" s="90"/>
       <c r="B40" s="155"/>
       <c r="M40" s="84"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" s="90"/>
       <c r="B41" s="155"/>
       <c r="M41" s="84"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="M42" s="84"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="M43" s="84"/>
     </row>
-    <row r="44" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M44" s="84"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="M45" s="84"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="M46" s="84"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="M47" s="84"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="M48" s="84"/>
     </row>
     <row r="49" spans="13:13" x14ac:dyDescent="0.2">
@@ -28502,9 +28669,11 @@
       <c r="K74" s="126"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="P8:P12"/>
     <mergeCell ref="P13:P18"/>
+    <mergeCell ref="R2:W2"/>
+    <mergeCell ref="W30:W34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -28517,6 +28686,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -28639,7 +28809,7 @@
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </to>
@@ -28661,6 +28831,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -28720,7 +28891,7 @@
               </from>
               <to>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>1933575</xdr:colOff>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>

</xml_diff>